<commit_message>
Added Florio et al. (2022) instances and updated excel file
The Excel file contains a single instance that was out of memory before the 1 hour mark. It has now been properly labeled.
</commit_message>
<xml_diff>
--- a/HoogendoornSpliet2024_FullResults/FullResults.xlsx
+++ b/HoogendoornSpliet2024_FullResults/FullResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bestanden\Eclipse\VRPSD_Assumptions\HoogendoornSpliet2024_FullResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF90F45-9346-4AB4-B946-AAEF10539BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1B75E1-D94F-421F-AA05-6A6E3D6B69F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jabali" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="331">
   <si>
     <t>VRPSD</t>
   </si>
@@ -1029,13 +1029,16 @@
   </si>
   <si>
     <t>Rec</t>
+  </si>
+  <si>
+    <t>Out of memory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1045,6 +1048,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1070,32 +1080,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1376,10 +1376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U298"/>
+  <dimension ref="A1:W298"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z294" sqref="Z294"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,36 +1395,36 @@
     <col min="18" max="21" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="3" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="3" t="s">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="3" t="s">
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>197855</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1570,20 +1570,23 @@
       <c r="P4" s="2">
         <v>242778</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" s="6">
         <v>666.56700000000001</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="6">
         <v>3248.12</v>
       </c>
-      <c r="T4" s="2">
-        <v>0</v>
-      </c>
-      <c r="U4" s="2">
+      <c r="T4" s="6">
+        <v>11.69</v>
+      </c>
+      <c r="U4" s="6">
         <v>289322</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W4" s="6" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1636,7 +1639,7 @@
         <v>192559</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -1689,7 +1692,7 @@
         <v>181226</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -1742,7 +1745,7 @@
         <v>174398</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1795,7 +1798,7 @@
         <v>174329</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -1848,7 +1851,7 @@
         <v>175542</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1901,7 +1904,7 @@
         <v>175021</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -1954,7 +1957,7 @@
         <v>186927</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -2007,7 +2010,7 @@
         <v>167763</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -2060,7 +2063,7 @@
         <v>170623</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -2113,7 +2116,7 @@
         <v>203063</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -15808,15 +15811,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="1.7109375" style="7" customWidth="1"/>
-    <col min="3" max="6" width="9.140625" style="7"/>
-    <col min="7" max="7" width="2.140625" style="7" customWidth="1"/>
-    <col min="8" max="11" width="9.140625" style="7"/>
-    <col min="12" max="12" width="1.42578125" style="7" customWidth="1"/>
-    <col min="13" max="16" width="9.140625" style="7"/>
-    <col min="17" max="17" width="1.5703125" style="7" customWidth="1"/>
-    <col min="18" max="21" width="9.140625" style="7"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.7109375" customWidth="1"/>
+    <col min="7" max="7" width="2.140625" customWidth="1"/>
+    <col min="12" max="12" width="1.42578125" customWidth="1"/>
+    <col min="17" max="17" width="1.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -15826,21 +15825,21 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
-      <c r="G1" s="6"/>
+      <c r="G1" s="1"/>
       <c r="H1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
-      <c r="L1" s="6"/>
+      <c r="L1" s="1"/>
       <c r="M1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
-      <c r="Q1" s="6"/>
+      <c r="Q1" s="1"/>
       <c r="R1" s="5" t="s">
         <v>3</v>
       </c>
@@ -15849,1751 +15848,1751 @@
       <c r="U1" s="5"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="S2" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="T2" t="s">
         <v>7</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="U2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" t="s">
         <v>279</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3">
         <v>332.75299999999999</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="E3" s="7">
-        <v>0</v>
-      </c>
-      <c r="F3" s="7">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>6</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3">
         <v>332.75299999999999</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="J3" s="7">
-        <v>0</v>
-      </c>
-      <c r="K3" s="7">
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
         <v>14</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3">
         <v>332.75299999999999</v>
       </c>
-      <c r="N3" s="7">
+      <c r="N3">
         <v>3.835</v>
       </c>
-      <c r="O3" s="7">
-        <v>0</v>
-      </c>
-      <c r="P3" s="7">
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
         <v>1594</v>
       </c>
-      <c r="R3" s="7">
+      <c r="R3">
         <v>332.47500000000002</v>
       </c>
-      <c r="S3" s="7">
+      <c r="S3">
         <v>224.53399999999999</v>
       </c>
-      <c r="T3" s="7">
-        <v>0</v>
-      </c>
-      <c r="U3" s="7">
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
         <v>30638</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" t="s">
         <v>280</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4">
         <v>335.29599999999999</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4">
         <v>0.13100000000000001</v>
       </c>
-      <c r="E4" s="7">
-        <v>0</v>
-      </c>
-      <c r="F4" s="7">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <v>15</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4">
         <v>335.29599999999999</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4">
         <v>0.21</v>
       </c>
-      <c r="J4" s="7">
-        <v>0</v>
-      </c>
-      <c r="K4" s="7">
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
         <v>60</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4">
         <v>335.29599999999999</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N4">
         <v>34.521999999999998</v>
       </c>
-      <c r="O4" s="7">
-        <v>0</v>
-      </c>
-      <c r="P4" s="7">
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
         <v>9796</v>
       </c>
-      <c r="R4" s="7">
+      <c r="R4">
         <v>335.21800000000002</v>
       </c>
-      <c r="S4" s="7">
+      <c r="S4">
         <v>1280.1600000000001</v>
       </c>
-      <c r="T4" s="7">
-        <v>0</v>
-      </c>
-      <c r="U4" s="7">
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
         <v>76613</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" t="s">
         <v>281</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5">
         <v>337.67399999999998</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5">
         <v>0.76200000000000001</v>
       </c>
-      <c r="E5" s="7">
-        <v>0</v>
-      </c>
-      <c r="F5" s="7">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>195</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5">
         <v>337.67399999999998</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5">
         <v>0.56599999999999995</v>
       </c>
-      <c r="J5" s="7">
-        <v>0</v>
-      </c>
-      <c r="K5" s="7">
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
         <v>175</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5">
         <v>337.67399999999998</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5">
         <v>88.950999999999993</v>
       </c>
-      <c r="O5" s="7">
-        <v>0</v>
-      </c>
-      <c r="P5" s="7">
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
         <v>15707</v>
       </c>
-      <c r="R5" s="7">
+      <c r="R5">
         <v>337.19799999999998</v>
       </c>
-      <c r="S5" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T5" s="7">
+      <c r="S5">
+        <v>3600</v>
+      </c>
+      <c r="T5">
         <v>1.3074300000000001</v>
       </c>
-      <c r="U5" s="7">
+      <c r="U5">
         <v>132133</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" t="s">
         <v>282</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6">
         <v>344.52499999999998</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6">
         <v>2.7879999999999998</v>
       </c>
-      <c r="E6" s="7">
-        <v>0</v>
-      </c>
-      <c r="F6" s="7">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>1100</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6">
         <v>344.52499999999998</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6">
         <v>3.105</v>
       </c>
-      <c r="J6" s="7">
-        <v>0</v>
-      </c>
-      <c r="K6" s="7">
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
         <v>1183</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6">
         <v>343.39299999999997</v>
       </c>
-      <c r="N6" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O6" s="7">
+      <c r="N6">
+        <v>3600</v>
+      </c>
+      <c r="O6">
         <v>1.1335900000000001</v>
       </c>
-      <c r="P6" s="7">
+      <c r="P6">
         <v>94584</v>
       </c>
-      <c r="R6" s="7">
+      <c r="R6">
         <v>343.20499999999998</v>
       </c>
-      <c r="S6" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T6" s="7">
+      <c r="S6">
+        <v>3600</v>
+      </c>
+      <c r="T6">
         <v>3.9932699999999999</v>
       </c>
-      <c r="U6" s="7">
+      <c r="U6">
         <v>109038</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" t="s">
         <v>283</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7">
         <v>358.947</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7">
         <v>0.21</v>
       </c>
-      <c r="E7" s="7">
-        <v>0</v>
-      </c>
-      <c r="F7" s="7">
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>49</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7">
         <v>358.947</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7">
         <v>0.16900000000000001</v>
       </c>
-      <c r="J7" s="7">
-        <v>0</v>
-      </c>
-      <c r="K7" s="7">
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
         <v>64</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7">
         <v>361.76400000000001</v>
       </c>
-      <c r="N7" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O7" s="7">
+      <c r="N7">
+        <v>3600</v>
+      </c>
+      <c r="O7">
         <v>4.6921799999999996</v>
       </c>
-      <c r="P7" s="7">
+      <c r="P7">
         <v>113974</v>
       </c>
-      <c r="R7" s="7">
+      <c r="R7">
         <v>359.99099999999999</v>
       </c>
-      <c r="S7" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T7" s="7">
+      <c r="S7">
+        <v>3600</v>
+      </c>
+      <c r="T7">
         <v>8.8866099999999992</v>
       </c>
-      <c r="U7" s="7">
+      <c r="U7">
         <v>141083</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" t="s">
         <v>284</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8">
         <v>364.06599999999997</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8">
         <v>0.89200000000000002</v>
       </c>
-      <c r="E8" s="7">
-        <v>0</v>
-      </c>
-      <c r="F8" s="7">
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>313</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8">
         <v>364.06599999999997</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8">
         <v>1.1020000000000001</v>
       </c>
-      <c r="J8" s="7">
-        <v>0</v>
-      </c>
-      <c r="K8" s="7">
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
         <v>455</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8">
         <v>371.91800000000001</v>
       </c>
-      <c r="N8" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O8" s="7">
+      <c r="N8">
+        <v>3600</v>
+      </c>
+      <c r="O8">
         <v>7.6140800000000004</v>
       </c>
-      <c r="P8" s="7">
+      <c r="P8">
         <v>121649</v>
       </c>
-      <c r="R8" s="7">
+      <c r="R8">
         <v>363.42500000000001</v>
       </c>
-      <c r="S8" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T8" s="7">
+      <c r="S8">
+        <v>3600</v>
+      </c>
+      <c r="T8">
         <v>9.7021200000000007</v>
       </c>
-      <c r="U8" s="7">
+      <c r="U8">
         <v>150627</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" t="s">
         <v>285</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9">
         <v>367.15499999999997</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9">
         <v>3.2010000000000001</v>
       </c>
-      <c r="E9" s="7">
-        <v>0</v>
-      </c>
-      <c r="F9" s="7">
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
         <v>1242</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9">
         <v>367.15499999999997</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9">
         <v>3.173</v>
       </c>
-      <c r="J9" s="7">
-        <v>0</v>
-      </c>
-      <c r="K9" s="7">
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
         <v>1274</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9">
         <v>370.37900000000002</v>
       </c>
-      <c r="N9" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O9" s="7">
+      <c r="N9">
+        <v>3600</v>
+      </c>
+      <c r="O9">
         <v>7.1220400000000001</v>
       </c>
-      <c r="P9" s="7">
+      <c r="P9">
         <v>107444</v>
       </c>
-      <c r="R9" s="7">
+      <c r="R9">
         <v>364.13200000000001</v>
       </c>
-      <c r="S9" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T9" s="7">
+      <c r="S9">
+        <v>3600</v>
+      </c>
+      <c r="T9">
         <v>10.0326</v>
       </c>
-      <c r="U9" s="7">
+      <c r="U9">
         <v>132410</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" t="s">
         <v>286</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10">
         <v>372.78399999999999</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10">
         <v>55.515000000000001</v>
       </c>
-      <c r="E10" s="7">
-        <v>0</v>
-      </c>
-      <c r="F10" s="7">
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
         <v>13374</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10">
         <v>372.78399999999999</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10">
         <v>57.576000000000001</v>
       </c>
-      <c r="J10" s="7">
-        <v>0</v>
-      </c>
-      <c r="K10" s="7">
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
         <v>13545</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10">
         <v>376.71899999999999</v>
       </c>
-      <c r="N10" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O10" s="7">
+      <c r="N10">
+        <v>3600</v>
+      </c>
+      <c r="O10">
         <v>8.9506700000000006</v>
       </c>
-      <c r="P10" s="7">
+      <c r="P10">
         <v>132310</v>
       </c>
-      <c r="R10" s="7">
+      <c r="R10">
         <v>374.04899999999998</v>
       </c>
-      <c r="S10" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T10" s="7">
+      <c r="S10">
+        <v>3600</v>
+      </c>
+      <c r="T10">
         <v>12.6973</v>
       </c>
-      <c r="U10" s="7">
+      <c r="U10">
         <v>144654</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" t="s">
         <v>287</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11">
         <v>441</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11">
         <v>0.47799999999999998</v>
       </c>
-      <c r="E11" s="7">
-        <v>0</v>
-      </c>
-      <c r="F11" s="7">
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
         <v>27</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11">
         <v>441</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11">
         <v>0.67800000000000005</v>
       </c>
-      <c r="J11" s="7">
-        <v>0</v>
-      </c>
-      <c r="K11" s="7">
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
         <v>74</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11">
         <v>441</v>
       </c>
-      <c r="N11" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O11" s="7">
+      <c r="N11">
+        <v>3600</v>
+      </c>
+      <c r="O11">
         <v>0.89196500000000001</v>
       </c>
-      <c r="P11" s="7">
+      <c r="P11">
         <v>94890</v>
       </c>
-      <c r="R11" s="7">
+      <c r="R11">
         <v>441</v>
       </c>
-      <c r="S11" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T11" s="7">
+      <c r="S11">
+        <v>3600</v>
+      </c>
+      <c r="T11">
         <v>2.00305</v>
       </c>
-      <c r="U11" s="7">
+      <c r="U11">
         <v>88067</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" t="s">
         <v>288</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12">
         <v>441.31099999999998</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12">
         <v>1.405</v>
       </c>
-      <c r="E12" s="7">
-        <v>0</v>
-      </c>
-      <c r="F12" s="7">
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
         <v>134</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12">
         <v>441.31099999999998</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12">
         <v>0.79700000000000004</v>
       </c>
-      <c r="J12" s="7">
-        <v>0</v>
-      </c>
-      <c r="K12" s="7">
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
         <v>102</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12">
         <v>441.31099999999998</v>
       </c>
-      <c r="N12" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O12" s="7">
+      <c r="N12">
+        <v>3600</v>
+      </c>
+      <c r="O12">
         <v>0.97593799999999997</v>
       </c>
-      <c r="P12" s="7">
+      <c r="P12">
         <v>98321</v>
       </c>
-      <c r="R12" s="7">
+      <c r="R12">
         <v>441.154</v>
       </c>
-      <c r="S12" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T12" s="7">
+      <c r="S12">
+        <v>3600</v>
+      </c>
+      <c r="T12">
         <v>1.99946</v>
       </c>
-      <c r="U12" s="7">
+      <c r="U12">
         <v>87347</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" t="s">
         <v>289</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13">
         <v>443.00599999999997</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13">
         <v>3.5310000000000001</v>
       </c>
-      <c r="E13" s="7">
-        <v>0</v>
-      </c>
-      <c r="F13" s="7">
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
         <v>493</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13">
         <v>443.00599999999997</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13">
         <v>5.141</v>
       </c>
-      <c r="J13" s="7">
-        <v>0</v>
-      </c>
-      <c r="K13" s="7">
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
         <v>762</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13">
         <v>443.11399999999998</v>
       </c>
-      <c r="N13" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O13" s="7">
+      <c r="N13">
+        <v>3600</v>
+      </c>
+      <c r="O13">
         <v>1.60544</v>
       </c>
-      <c r="P13" s="7">
+      <c r="P13">
         <v>66251</v>
       </c>
-      <c r="R13" s="7">
+      <c r="R13">
         <v>442.35899999999998</v>
       </c>
-      <c r="S13" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T13" s="7">
+      <c r="S13">
+        <v>3600</v>
+      </c>
+      <c r="T13">
         <v>2.3842500000000002</v>
       </c>
-      <c r="U13" s="7">
+      <c r="U13">
         <v>63980</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" t="s">
         <v>290</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14">
         <v>448.08300000000003</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14">
         <v>189.203</v>
       </c>
-      <c r="E14" s="7">
-        <v>0</v>
-      </c>
-      <c r="F14" s="7">
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
         <v>16969</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14">
         <v>448.08300000000003</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14">
         <v>186.14</v>
       </c>
-      <c r="J14" s="7">
-        <v>0</v>
-      </c>
-      <c r="K14" s="7">
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
         <v>17143</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M14">
         <v>449.149</v>
       </c>
-      <c r="N14" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O14" s="7">
+      <c r="N14">
+        <v>3600</v>
+      </c>
+      <c r="O14">
         <v>3.1501399999999999</v>
       </c>
-      <c r="P14" s="7">
+      <c r="P14">
         <v>67142</v>
       </c>
-      <c r="R14" s="7">
+      <c r="R14">
         <v>446.61599999999999</v>
       </c>
-      <c r="S14" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T14" s="7">
+      <c r="S14">
+        <v>3600</v>
+      </c>
+      <c r="T14">
         <v>3.4591799999999999</v>
       </c>
-      <c r="U14" s="7">
+      <c r="U14">
         <v>57246</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" t="s">
         <v>291</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15">
         <v>459</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15">
         <v>0.48899999999999999</v>
       </c>
-      <c r="E15" s="7">
-        <v>0</v>
-      </c>
-      <c r="F15" s="7">
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
         <v>24</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15">
         <v>459</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15">
         <v>0.38400000000000001</v>
       </c>
-      <c r="J15" s="7">
-        <v>0</v>
-      </c>
-      <c r="K15" s="7">
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
         <v>21</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M15">
         <v>464</v>
       </c>
-      <c r="N15" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O15" s="7">
+      <c r="N15">
+        <v>3600</v>
+      </c>
+      <c r="O15">
         <v>4.3642200000000004</v>
       </c>
-      <c r="P15" s="7">
+      <c r="P15">
         <v>92821</v>
       </c>
-      <c r="R15" s="7">
+      <c r="R15">
         <v>460.00200000000001</v>
       </c>
-      <c r="S15" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T15" s="7">
+      <c r="S15">
+        <v>3600</v>
+      </c>
+      <c r="T15">
         <v>6.2481</v>
       </c>
-      <c r="U15" s="7">
+      <c r="U15">
         <v>84883</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" t="s">
         <v>292</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16">
         <v>459.04899999999998</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16">
         <v>1.0029999999999999</v>
       </c>
-      <c r="E16" s="7">
-        <v>0</v>
-      </c>
-      <c r="F16" s="7">
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
         <v>89</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16">
         <v>459.04899999999998</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16">
         <v>0.45100000000000001</v>
       </c>
-      <c r="J16" s="7">
-        <v>0</v>
-      </c>
-      <c r="K16" s="7">
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
         <v>24</v>
       </c>
-      <c r="M16" s="7">
+      <c r="M16">
         <v>466.01</v>
       </c>
-      <c r="N16" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O16" s="7">
+      <c r="N16">
+        <v>3600</v>
+      </c>
+      <c r="O16">
         <v>4.6158200000000003</v>
       </c>
-      <c r="P16" s="7">
+      <c r="P16">
         <v>89964</v>
       </c>
-      <c r="R16" s="7">
+      <c r="R16">
         <v>462.22899999999998</v>
       </c>
-      <c r="S16" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T16" s="7">
+      <c r="S16">
+        <v>3600</v>
+      </c>
+      <c r="T16">
         <v>6.8898200000000003</v>
       </c>
-      <c r="U16" s="7">
+      <c r="U16">
         <v>85392</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" t="s">
         <v>293</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17">
         <v>460.55</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17">
         <v>1.7829999999999999</v>
       </c>
-      <c r="E17" s="7">
-        <v>0</v>
-      </c>
-      <c r="F17" s="7">
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
         <v>216</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17">
         <v>460.55</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17">
         <v>1.335</v>
       </c>
-      <c r="J17" s="7">
-        <v>0</v>
-      </c>
-      <c r="K17" s="7">
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
         <v>156</v>
       </c>
-      <c r="M17" s="7">
+      <c r="M17">
         <v>470.892</v>
       </c>
-      <c r="N17" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O17" s="7">
+      <c r="N17">
+        <v>3600</v>
+      </c>
+      <c r="O17">
         <v>5.8170200000000003</v>
       </c>
-      <c r="P17" s="7">
+      <c r="P17">
         <v>87391</v>
       </c>
-      <c r="R17" s="7">
+      <c r="R17">
         <v>461.37299999999999</v>
       </c>
-      <c r="S17" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T17" s="7">
+      <c r="S17">
+        <v>3600</v>
+      </c>
+      <c r="T17">
         <v>6.5831799999999996</v>
       </c>
-      <c r="U17" s="7">
+      <c r="U17">
         <v>61532</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" t="s">
         <v>294</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18">
         <v>465.62900000000002</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18">
         <v>34.274999999999999</v>
       </c>
-      <c r="E18" s="7">
-        <v>0</v>
-      </c>
-      <c r="F18" s="7">
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
         <v>3469</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18">
         <v>465.62900000000002</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18">
         <v>41.737000000000002</v>
       </c>
-      <c r="J18" s="7">
-        <v>0</v>
-      </c>
-      <c r="K18" s="7">
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
         <v>4224</v>
       </c>
-      <c r="M18" s="7">
+      <c r="M18">
         <v>473.32100000000003</v>
       </c>
-      <c r="N18" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O18" s="7">
+      <c r="N18">
+        <v>3600</v>
+      </c>
+      <c r="O18">
         <v>6.3003299999999998</v>
       </c>
-      <c r="P18" s="7">
+      <c r="P18">
         <v>84852</v>
       </c>
-      <c r="R18" s="7">
+      <c r="R18">
         <v>466.52300000000002</v>
       </c>
-      <c r="S18" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T18" s="7">
+      <c r="S18">
+        <v>3600</v>
+      </c>
+      <c r="T18">
         <v>7.8194600000000003</v>
       </c>
-      <c r="U18" s="7">
+      <c r="U18">
         <v>60997</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" t="s">
         <v>295</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19">
         <v>549.005</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19">
         <v>0.92600000000000005</v>
       </c>
-      <c r="E19" s="7">
-        <v>0</v>
-      </c>
-      <c r="F19" s="7">
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
         <v>9</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19">
         <v>549.005</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19">
         <v>0.52800000000000002</v>
       </c>
-      <c r="J19" s="7">
-        <v>0</v>
-      </c>
-      <c r="K19" s="7">
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
         <v>10</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M19">
         <v>555.00300000000004</v>
       </c>
-      <c r="N19" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O19" s="7">
+      <c r="N19">
+        <v>3600</v>
+      </c>
+      <c r="O19">
         <v>2.07057</v>
       </c>
-      <c r="P19" s="7">
+      <c r="P19">
         <v>44073</v>
       </c>
-      <c r="R19" s="7">
+      <c r="R19">
         <v>549.00400000000002</v>
       </c>
-      <c r="S19" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T19" s="7">
+      <c r="S19">
+        <v>3600</v>
+      </c>
+      <c r="T19">
         <v>1.8221700000000001</v>
       </c>
-      <c r="U19" s="7">
+      <c r="U19">
         <v>33891</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" t="s">
         <v>296</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20">
         <v>550.16399999999999</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20">
         <v>3.6520000000000001</v>
       </c>
-      <c r="E20" s="7">
-        <v>0</v>
-      </c>
-      <c r="F20" s="7">
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
         <v>113</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20">
         <v>550.16399999999999</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20">
         <v>3.63</v>
       </c>
-      <c r="J20" s="7">
-        <v>0</v>
-      </c>
-      <c r="K20" s="7">
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
         <v>131</v>
       </c>
-      <c r="M20" s="7">
+      <c r="M20">
         <v>562.87199999999996</v>
       </c>
-      <c r="N20" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O20" s="7">
+      <c r="N20">
+        <v>3600</v>
+      </c>
+      <c r="O20">
         <v>3.41194</v>
       </c>
-      <c r="P20" s="7">
+      <c r="P20">
         <v>42286</v>
       </c>
-      <c r="R20" s="7">
+      <c r="R20">
         <v>553.48</v>
       </c>
-      <c r="S20" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T20" s="7">
+      <c r="S20">
+        <v>3600</v>
+      </c>
+      <c r="T20">
         <v>2.7064699999999999</v>
       </c>
-      <c r="U20" s="7">
+      <c r="U20">
         <v>35245</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" t="s">
         <v>297</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21">
         <v>550.81500000000005</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21">
         <v>6.4269999999999996</v>
       </c>
-      <c r="E21" s="7">
-        <v>0</v>
-      </c>
-      <c r="F21" s="7">
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
         <v>159</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21">
         <v>550.81500000000005</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21">
         <v>5.1079999999999997</v>
       </c>
-      <c r="J21" s="7">
-        <v>0</v>
-      </c>
-      <c r="K21" s="7">
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
         <v>167</v>
       </c>
-      <c r="M21" s="7">
+      <c r="M21">
         <v>552.83000000000004</v>
       </c>
-      <c r="N21" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O21" s="7">
+      <c r="N21">
+        <v>3600</v>
+      </c>
+      <c r="O21">
         <v>1.6867399999999999</v>
       </c>
-      <c r="P21" s="7">
+      <c r="P21">
         <v>26792</v>
       </c>
-      <c r="R21" s="7">
+      <c r="R21">
         <v>555.89800000000002</v>
       </c>
-      <c r="S21" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T21" s="7">
+      <c r="S21">
+        <v>3600</v>
+      </c>
+      <c r="T21">
         <v>3.1541899999999998</v>
       </c>
-      <c r="U21" s="7">
+      <c r="U21">
         <v>18954</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" t="s">
         <v>298</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22">
         <v>554.79999999999995</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22">
         <v>325.07600000000002</v>
       </c>
-      <c r="E22" s="7">
-        <v>0</v>
-      </c>
-      <c r="F22" s="7">
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
         <v>11016</v>
       </c>
-      <c r="H22" s="7">
+      <c r="H22">
         <v>554.79999999999995</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22">
         <v>346.84</v>
       </c>
-      <c r="J22" s="7">
-        <v>0</v>
-      </c>
-      <c r="K22" s="7">
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
         <v>11490</v>
       </c>
-      <c r="M22" s="7">
+      <c r="M22">
         <v>574.23599999999999</v>
       </c>
-      <c r="N22" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O22" s="7">
+      <c r="N22">
+        <v>3600</v>
+      </c>
+      <c r="O22">
         <v>5.3890399999999996</v>
       </c>
-      <c r="P22" s="7">
+      <c r="P22">
         <v>26590</v>
       </c>
-      <c r="R22" s="7">
+      <c r="R22">
         <v>563.43200000000002</v>
       </c>
-      <c r="S22" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T22" s="7">
+      <c r="S22">
+        <v>3600</v>
+      </c>
+      <c r="T22">
         <v>4.4503399999999997</v>
       </c>
-      <c r="U22" s="7">
+      <c r="U22">
         <v>19566</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" t="s">
         <v>299</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23">
         <v>567.12599999999998</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23">
         <v>16.225999999999999</v>
       </c>
-      <c r="E23" s="7">
-        <v>0</v>
-      </c>
-      <c r="F23" s="7">
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
         <v>746</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23">
         <v>567.12599999999998</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23">
         <v>17.244</v>
       </c>
-      <c r="J23" s="7">
-        <v>0</v>
-      </c>
-      <c r="K23" s="7">
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
         <v>540</v>
       </c>
-      <c r="M23" s="7">
+      <c r="M23">
         <v>596.05200000000002</v>
       </c>
-      <c r="N23" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O23" s="7">
+      <c r="N23">
+        <v>3600</v>
+      </c>
+      <c r="O23">
         <v>7.7262500000000003</v>
       </c>
-      <c r="P23" s="7">
+      <c r="P23">
         <v>49257</v>
       </c>
-      <c r="R23" s="7">
+      <c r="R23">
         <v>586.05200000000002</v>
       </c>
-      <c r="S23" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T23" s="7">
+      <c r="S23">
+        <v>3600</v>
+      </c>
+      <c r="T23">
         <v>7.9390299999999998</v>
       </c>
-      <c r="U23" s="7">
+      <c r="U23">
         <v>36095</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" t="s">
         <v>300</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24">
         <v>569.26599999999996</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24">
         <v>59.287999999999997</v>
       </c>
-      <c r="E24" s="7">
-        <v>0</v>
-      </c>
-      <c r="F24" s="7">
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
         <v>1669</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24">
         <v>569.26599999999996</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24">
         <v>58.151000000000003</v>
       </c>
-      <c r="J24" s="7">
-        <v>0</v>
-      </c>
-      <c r="K24" s="7">
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
         <v>1632</v>
       </c>
-      <c r="M24" s="7">
+      <c r="M24">
         <v>588.327</v>
       </c>
-      <c r="N24" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O24" s="7">
+      <c r="N24">
+        <v>3600</v>
+      </c>
+      <c r="O24">
         <v>6.5263</v>
       </c>
-      <c r="P24" s="7">
+      <c r="P24">
         <v>48979</v>
       </c>
-      <c r="R24" s="7">
+      <c r="R24">
         <v>587.673</v>
       </c>
-      <c r="S24" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T24" s="7">
+      <c r="S24">
+        <v>3600</v>
+      </c>
+      <c r="T24">
         <v>8.1759400000000007</v>
       </c>
-      <c r="U24" s="7">
+      <c r="U24">
         <v>37457</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" t="s">
         <v>301</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25">
         <v>569.952</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25">
         <v>120.40900000000001</v>
       </c>
-      <c r="E25" s="7">
-        <v>0</v>
-      </c>
-      <c r="F25" s="7">
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
         <v>4376</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H25">
         <v>569.952</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25">
         <v>82.545000000000002</v>
       </c>
-      <c r="J25" s="7">
-        <v>0</v>
-      </c>
-      <c r="K25" s="7">
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
         <v>3379</v>
       </c>
-      <c r="M25" s="7">
+      <c r="M25">
         <v>595.17499999999995</v>
       </c>
-      <c r="N25" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O25" s="7">
+      <c r="N25">
+        <v>3600</v>
+      </c>
+      <c r="O25">
         <v>7.6928099999999997</v>
       </c>
-      <c r="P25" s="7">
+      <c r="P25">
         <v>35851</v>
       </c>
-      <c r="R25" s="7">
+      <c r="R25">
         <v>588.39200000000005</v>
       </c>
-      <c r="S25" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T25" s="7">
+      <c r="S25">
+        <v>3600</v>
+      </c>
+      <c r="T25">
         <v>8.3519500000000004</v>
       </c>
-      <c r="U25" s="7">
+      <c r="U25">
         <v>22113</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" t="s">
         <v>302</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26">
         <v>573.25</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26">
         <v>1410.84</v>
       </c>
-      <c r="E26" s="7">
-        <v>0</v>
-      </c>
-      <c r="F26" s="7">
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
         <v>24180</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26">
         <v>573.25</v>
       </c>
-      <c r="I26" s="7">
+      <c r="I26">
         <v>797.4</v>
       </c>
-      <c r="J26" s="7">
-        <v>0</v>
-      </c>
-      <c r="K26" s="7">
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
         <v>17117</v>
       </c>
-      <c r="M26" s="7">
+      <c r="M26">
         <v>600.55899999999997</v>
       </c>
-      <c r="N26" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O26" s="7">
+      <c r="N26">
+        <v>3600</v>
+      </c>
+      <c r="O26">
         <v>8.5185999999999993</v>
       </c>
-      <c r="P26" s="7">
+      <c r="P26">
         <v>40646</v>
       </c>
-      <c r="R26" s="7">
+      <c r="R26">
         <v>590.34100000000001</v>
       </c>
-      <c r="S26" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T26" s="7">
+      <c r="S26">
+        <v>3600</v>
+      </c>
+      <c r="T26">
         <v>8.6403099999999995</v>
       </c>
-      <c r="U26" s="7">
+      <c r="U26">
         <v>22816</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" t="s">
         <v>303</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27">
         <v>640.00099999999998</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27">
         <v>3.0289999999999999</v>
       </c>
-      <c r="E27" s="7">
-        <v>0</v>
-      </c>
-      <c r="F27" s="7">
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
         <v>31</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H27">
         <v>640.00099999999998</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27">
         <v>0.94199999999999995</v>
       </c>
-      <c r="J27" s="7">
-        <v>0</v>
-      </c>
-      <c r="K27" s="7">
-        <v>0</v>
-      </c>
-      <c r="M27" s="7">
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="M27">
         <v>641.01900000000001</v>
       </c>
-      <c r="N27" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O27" s="7">
+      <c r="N27">
+        <v>3600</v>
+      </c>
+      <c r="O27">
         <v>0.93892399999999998</v>
       </c>
-      <c r="P27" s="7">
+      <c r="P27">
         <v>22118</v>
       </c>
-      <c r="R27" s="7">
+      <c r="R27">
         <v>641.01700000000005</v>
       </c>
-      <c r="S27" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T27" s="7">
+      <c r="S27">
+        <v>3600</v>
+      </c>
+      <c r="T27">
         <v>1.53975</v>
       </c>
-      <c r="U27" s="7">
+      <c r="U27">
         <v>15802</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" t="s">
         <v>304</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28">
         <v>641.73199999999997</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28">
         <v>22.32</v>
       </c>
-      <c r="E28" s="7">
-        <v>0</v>
-      </c>
-      <c r="F28" s="7">
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
         <v>476</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28">
         <v>641.73199999999997</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28">
         <v>58.366999999999997</v>
       </c>
-      <c r="J28" s="7">
-        <v>0</v>
-      </c>
-      <c r="K28" s="7">
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
         <v>1179</v>
       </c>
-      <c r="M28" s="7">
+      <c r="M28">
         <v>644.86800000000005</v>
       </c>
-      <c r="N28" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O28" s="7">
+      <c r="N28">
+        <v>3600</v>
+      </c>
+      <c r="O28">
         <v>1.53026</v>
       </c>
-      <c r="P28" s="7">
+      <c r="P28">
         <v>22010</v>
       </c>
-      <c r="R28" s="7">
+      <c r="R28">
         <v>641.40200000000004</v>
       </c>
-      <c r="S28" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T28" s="7">
+      <c r="S28">
+        <v>3600</v>
+      </c>
+      <c r="T28">
         <v>1.5722400000000001</v>
       </c>
-      <c r="U28" s="7">
+      <c r="U28">
         <v>15533</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="A29" t="s">
         <v>305</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29">
         <v>641.30399999999997</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29">
         <v>300.90100000000001</v>
       </c>
-      <c r="E29" s="7">
-        <v>0</v>
-      </c>
-      <c r="F29" s="7">
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
         <v>3086</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H29">
         <v>641.30399999999997</v>
       </c>
-      <c r="I29" s="7">
+      <c r="I29">
         <v>133.25800000000001</v>
       </c>
-      <c r="J29" s="7">
-        <v>0</v>
-      </c>
-      <c r="K29" s="7">
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
         <v>1273</v>
       </c>
-      <c r="M29" s="7">
+      <c r="M29">
         <v>644.93899999999996</v>
       </c>
-      <c r="N29" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O29" s="7">
+      <c r="N29">
+        <v>3600</v>
+      </c>
+      <c r="O29">
         <v>1.7808999999999999</v>
       </c>
-      <c r="P29" s="7">
+      <c r="P29">
         <v>11321</v>
       </c>
-      <c r="R29" s="7">
+      <c r="R29">
         <v>642.70399999999995</v>
       </c>
-      <c r="S29" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T29" s="7">
+      <c r="S29">
+        <v>3600</v>
+      </c>
+      <c r="T29">
         <v>1.8988</v>
       </c>
-      <c r="U29" s="7">
+      <c r="U29">
         <v>8472</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" t="s">
         <v>306</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30">
         <v>646.11900000000003</v>
       </c>
-      <c r="D30" s="7">
-        <v>3600</v>
-      </c>
-      <c r="E30" s="7">
+      <c r="D30">
+        <v>3600</v>
+      </c>
+      <c r="E30">
         <v>0.38215700000000002</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30">
         <v>27193</v>
       </c>
-      <c r="H30" s="7">
+      <c r="H30">
         <v>646.11900000000003</v>
       </c>
-      <c r="I30" s="7">
-        <v>3600</v>
-      </c>
-      <c r="J30" s="7">
+      <c r="I30">
+        <v>3600</v>
+      </c>
+      <c r="J30">
         <v>0.434975</v>
       </c>
-      <c r="K30" s="7">
+      <c r="K30">
         <v>22946</v>
       </c>
-      <c r="M30" s="7">
+      <c r="M30">
         <v>649.23299999999995</v>
       </c>
-      <c r="N30" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O30" s="7">
+      <c r="N30">
+        <v>3600</v>
+      </c>
+      <c r="O30">
         <v>2.29691</v>
       </c>
-      <c r="P30" s="7">
+      <c r="P30">
         <v>10319</v>
       </c>
-      <c r="R30" s="7">
+      <c r="R30">
         <v>646.37599999999998</v>
       </c>
-      <c r="S30" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T30" s="7">
+      <c r="S30">
+        <v>3600</v>
+      </c>
+      <c r="T30">
         <v>2.3415300000000001</v>
       </c>
-      <c r="U30" s="7">
+      <c r="U30">
         <v>9130</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+      <c r="A31" t="s">
         <v>307</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31">
         <v>655.35400000000004</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31">
         <v>7.0919999999999996</v>
       </c>
-      <c r="E31" s="7">
-        <v>0</v>
-      </c>
-      <c r="F31" s="7">
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
         <v>141</v>
       </c>
-      <c r="H31" s="7">
+      <c r="H31">
         <v>655.35400000000004</v>
       </c>
-      <c r="I31" s="7">
+      <c r="I31">
         <v>7.8250000000000002</v>
       </c>
-      <c r="J31" s="7">
-        <v>0</v>
-      </c>
-      <c r="K31" s="7">
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
         <v>199</v>
       </c>
-      <c r="M31" s="7">
+      <c r="M31">
         <v>662.35400000000004</v>
       </c>
-      <c r="N31" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O31" s="7">
+      <c r="N31">
+        <v>3600</v>
+      </c>
+      <c r="O31">
         <v>2.7710599999999999</v>
       </c>
-      <c r="P31" s="7">
+      <c r="P31">
         <v>21872</v>
       </c>
-      <c r="R31" s="7">
+      <c r="R31">
         <v>673.92600000000004</v>
       </c>
-      <c r="S31" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T31" s="7">
+      <c r="S31">
+        <v>3600</v>
+      </c>
+      <c r="T31">
         <v>6.3250599999999997</v>
       </c>
-      <c r="U31" s="7">
+      <c r="U31">
         <v>17465</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="A32" t="s">
         <v>308</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32">
         <v>658.29700000000003</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32">
         <v>92.581999999999994</v>
       </c>
-      <c r="E32" s="7">
-        <v>0</v>
-      </c>
-      <c r="F32" s="7">
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
         <v>2184</v>
       </c>
-      <c r="H32" s="7">
+      <c r="H32">
         <v>658.29700000000003</v>
       </c>
-      <c r="I32" s="7">
+      <c r="I32">
         <v>87.078999999999994</v>
       </c>
-      <c r="J32" s="7">
-        <v>0</v>
-      </c>
-      <c r="K32" s="7">
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
         <v>1532</v>
       </c>
-      <c r="M32" s="7">
+      <c r="M32">
         <v>671.22799999999995</v>
       </c>
-      <c r="N32" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O32" s="7">
+      <c r="N32">
+        <v>3600</v>
+      </c>
+      <c r="O32">
         <v>4.1309300000000002</v>
       </c>
-      <c r="P32" s="7">
+      <c r="P32">
         <v>22625</v>
       </c>
-      <c r="R32" s="7">
+      <c r="R32">
         <v>663.678</v>
       </c>
-      <c r="S32" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T32" s="7">
+      <c r="S32">
+        <v>3600</v>
+      </c>
+      <c r="T32">
         <v>4.9615</v>
       </c>
-      <c r="U32" s="7">
+      <c r="U32">
         <v>17055</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="A33" t="s">
         <v>309</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33">
         <v>658.98400000000004</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33">
         <v>162.13200000000001</v>
       </c>
-      <c r="E33" s="7">
-        <v>0</v>
-      </c>
-      <c r="F33" s="7">
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
         <v>3089</v>
       </c>
-      <c r="H33" s="7">
+      <c r="H33">
         <v>658.98400000000004</v>
       </c>
-      <c r="I33" s="7">
+      <c r="I33">
         <v>175.851</v>
       </c>
-      <c r="J33" s="7">
-        <v>0</v>
-      </c>
-      <c r="K33" s="7">
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
         <v>3514</v>
       </c>
-      <c r="M33" s="7">
+      <c r="M33">
         <v>671.27700000000004</v>
       </c>
-      <c r="N33" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O33" s="7">
+      <c r="N33">
+        <v>3600</v>
+      </c>
+      <c r="O33">
         <v>4.1975199999999999</v>
       </c>
-      <c r="P33" s="7">
+      <c r="P33">
         <v>14392</v>
       </c>
-      <c r="R33" s="7">
+      <c r="R33">
         <v>671.529</v>
       </c>
-      <c r="S33" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T33" s="7">
+      <c r="S33">
+        <v>3600</v>
+      </c>
+      <c r="T33">
         <v>6.0047499999999996</v>
       </c>
-      <c r="U33" s="7">
+      <c r="U33">
         <v>9419</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="A34" t="s">
         <v>310</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34">
         <v>666.55499999999995</v>
       </c>
-      <c r="D34" s="7">
-        <v>3600</v>
-      </c>
-      <c r="E34" s="7">
+      <c r="D34">
+        <v>3600</v>
+      </c>
+      <c r="E34">
         <v>0.98324999999999996</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34">
         <v>24521</v>
       </c>
-      <c r="H34" s="7">
+      <c r="H34">
         <v>666.55499999999995</v>
       </c>
-      <c r="I34" s="7">
-        <v>3600</v>
-      </c>
-      <c r="J34" s="7">
+      <c r="I34">
+        <v>3600</v>
+      </c>
+      <c r="J34">
         <v>0.98336599999999996</v>
       </c>
-      <c r="K34" s="7">
+      <c r="K34">
         <v>24903</v>
       </c>
-      <c r="M34" s="7">
+      <c r="M34">
         <v>676.08500000000004</v>
       </c>
-      <c r="N34" s="7">
-        <v>3600</v>
-      </c>
-      <c r="O34" s="7">
+      <c r="N34">
+        <v>3600</v>
+      </c>
+      <c r="O34">
         <v>4.8674799999999996</v>
       </c>
-      <c r="P34" s="7">
+      <c r="P34">
         <v>13369</v>
       </c>
-      <c r="R34" s="7">
+      <c r="R34">
         <v>669.10299999999995</v>
       </c>
-      <c r="S34" s="7">
-        <v>3600</v>
-      </c>
-      <c r="T34" s="7">
+      <c r="S34">
+        <v>3600</v>
+      </c>
+      <c r="T34">
         <v>5.6261400000000004</v>
       </c>
-      <c r="U34" s="7">
+      <c r="U34">
         <v>10659</v>
       </c>
     </row>
@@ -17618,838 +17617,834 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="1.7109375" style="8" customWidth="1"/>
-    <col min="3" max="6" width="9.140625" style="8"/>
-    <col min="7" max="7" width="2.140625" style="8" customWidth="1"/>
-    <col min="8" max="11" width="9.140625" style="8"/>
-    <col min="12" max="12" width="1.42578125" style="8" customWidth="1"/>
-    <col min="13" max="16" width="9.140625" style="8"/>
-    <col min="17" max="17" width="1.5703125" style="8" customWidth="1"/>
-    <col min="18" max="21" width="9.140625" style="8"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.7109375" customWidth="1"/>
+    <col min="7" max="7" width="2.140625" customWidth="1"/>
+    <col min="12" max="12" width="1.42578125" customWidth="1"/>
+    <col min="17" max="17" width="1.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="9" t="s">
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="9" t="s">
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="9" t="s">
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="R2" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="S2" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="T2" t="s">
         <v>7</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="U2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" t="s">
         <v>311</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3">
         <v>710.11699999999996</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3">
         <v>1296.31</v>
       </c>
-      <c r="E3" s="8">
-        <v>0</v>
-      </c>
-      <c r="F3" s="8">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>56171</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3">
         <v>710.11699999999996</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3">
         <v>1498.1</v>
       </c>
-      <c r="J3" s="8">
-        <v>0</v>
-      </c>
-      <c r="K3" s="8">
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
         <v>67323</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3">
         <v>732.88300000000004</v>
       </c>
-      <c r="N3" s="8">
-        <v>3600</v>
-      </c>
-      <c r="O3" s="8">
+      <c r="N3">
+        <v>3600</v>
+      </c>
+      <c r="O3">
         <v>20.389900000000001</v>
       </c>
-      <c r="P3" s="8">
+      <c r="P3">
         <v>106993</v>
       </c>
-      <c r="R3" s="8">
+      <c r="R3">
         <v>719.55700000000002</v>
       </c>
-      <c r="S3" s="8">
-        <v>3600</v>
-      </c>
-      <c r="T3" s="8">
+      <c r="S3">
+        <v>3600</v>
+      </c>
+      <c r="T3">
         <v>26.490100000000002</v>
       </c>
-      <c r="U3" s="8">
+      <c r="U3">
         <v>49364</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" t="s">
         <v>312</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4">
         <v>254.21700000000001</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4">
         <v>12.260999999999999</v>
       </c>
-      <c r="E4" s="8">
-        <v>0</v>
-      </c>
-      <c r="F4" s="8">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <v>46</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4">
         <v>254.21700000000001</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4">
         <v>25.326000000000001</v>
       </c>
-      <c r="J4" s="8">
-        <v>0</v>
-      </c>
-      <c r="K4" s="8">
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
         <v>62</v>
       </c>
-      <c r="M4" s="8">
+      <c r="M4">
         <v>268.553</v>
       </c>
-      <c r="N4" s="8">
-        <v>3600</v>
-      </c>
-      <c r="O4" s="8">
+      <c r="N4">
+        <v>3600</v>
+      </c>
+      <c r="O4">
         <v>8.3980599999999992</v>
       </c>
-      <c r="P4" s="8">
+      <c r="P4">
         <v>7415</v>
       </c>
-      <c r="R4" s="8">
+      <c r="R4">
         <v>240.92400000000001</v>
       </c>
-      <c r="S4" s="8">
-        <v>3600</v>
-      </c>
-      <c r="T4" s="8">
+      <c r="S4">
+        <v>3600</v>
+      </c>
+      <c r="T4">
         <v>31.375299999999999</v>
       </c>
-      <c r="U4" s="8">
+      <c r="U4">
         <v>713</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" t="s">
         <v>313</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5">
         <v>377.38400000000001</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5">
         <v>0.5</v>
       </c>
-      <c r="E5" s="8">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8">
-        <v>0</v>
-      </c>
-      <c r="H5" s="8">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>377.38400000000001</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5">
         <v>1.369</v>
       </c>
-      <c r="J5" s="8">
-        <v>0</v>
-      </c>
-      <c r="K5" s="8">
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
         <v>7</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5">
         <v>417.447</v>
       </c>
-      <c r="N5" s="8">
-        <v>3600</v>
-      </c>
-      <c r="O5" s="8">
+      <c r="N5">
+        <v>3600</v>
+      </c>
+      <c r="O5">
         <v>21.133600000000001</v>
       </c>
-      <c r="P5" s="8">
+      <c r="P5">
         <v>1843</v>
       </c>
-      <c r="R5" s="8">
+      <c r="R5">
         <v>377.637</v>
       </c>
-      <c r="S5" s="8">
-        <v>3600</v>
-      </c>
-      <c r="T5" s="8">
+      <c r="S5">
+        <v>3600</v>
+      </c>
+      <c r="T5">
         <v>25.232600000000001</v>
       </c>
-      <c r="U5" s="8">
+      <c r="U5">
         <v>619</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" t="s">
         <v>314</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6">
         <v>569.27200000000005</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6">
         <v>0.46600000000000003</v>
       </c>
-      <c r="E6" s="8">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8">
-        <v>0</v>
-      </c>
-      <c r="H6" s="8">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>569.27200000000005</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6">
         <v>0.85099999999999998</v>
       </c>
-      <c r="J6" s="8">
-        <v>0</v>
-      </c>
-      <c r="K6" s="8">
-        <v>0</v>
-      </c>
-      <c r="M6" s="8">
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="M6">
         <v>583.61199999999997</v>
       </c>
-      <c r="N6" s="8">
-        <v>3600</v>
-      </c>
-      <c r="O6" s="8">
+      <c r="N6">
+        <v>3600</v>
+      </c>
+      <c r="O6">
         <v>8.8260900000000007</v>
       </c>
-      <c r="P6" s="8">
+      <c r="P6">
         <v>2388</v>
       </c>
-      <c r="R6" s="8">
+      <c r="R6">
         <v>571.43700000000001</v>
       </c>
-      <c r="S6" s="8">
-        <v>3600</v>
-      </c>
-      <c r="T6" s="8">
+      <c r="S6">
+        <v>3600</v>
+      </c>
+      <c r="T6">
         <v>15.478</v>
       </c>
-      <c r="U6" s="8">
+      <c r="U6">
         <v>665</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" t="s">
         <v>315</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7">
         <v>541.16700000000003</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7">
         <v>1115.27</v>
       </c>
-      <c r="E7" s="8">
-        <v>0</v>
-      </c>
-      <c r="F7" s="8">
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>1417</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7">
         <v>505.01100000000002</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7">
         <v>1.1359999999999999</v>
       </c>
-      <c r="J7" s="8">
-        <v>0</v>
-      </c>
-      <c r="K7" s="8">
-        <v>0</v>
-      </c>
-      <c r="M7" s="8">
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="M7">
         <v>523.41700000000003</v>
       </c>
-      <c r="N7" s="8">
-        <v>3600</v>
-      </c>
-      <c r="O7" s="8">
+      <c r="N7">
+        <v>3600</v>
+      </c>
+      <c r="O7">
         <v>18.482600000000001</v>
       </c>
-      <c r="P7" s="8">
+      <c r="P7">
         <v>1690</v>
       </c>
-      <c r="R7" s="8">
+      <c r="R7">
         <v>516.75300000000004</v>
       </c>
-      <c r="S7" s="8">
-        <v>3600</v>
-      </c>
-      <c r="T7" s="8">
+      <c r="S7">
+        <v>3600</v>
+      </c>
+      <c r="T7">
         <v>24.117799999999999</v>
       </c>
-      <c r="U7" s="8">
+      <c r="U7">
         <v>633</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" t="s">
         <v>316</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8">
         <v>407.99799999999999</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8">
         <v>272.27100000000002</v>
       </c>
-      <c r="E8" s="8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="8">
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>13558</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8">
         <v>407.99799999999999</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8">
         <v>464.60700000000003</v>
       </c>
-      <c r="J8" s="8">
-        <v>0</v>
-      </c>
-      <c r="K8" s="8">
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
         <v>19347</v>
       </c>
-      <c r="M8" s="8">
+      <c r="M8">
         <v>456.26900000000001</v>
       </c>
-      <c r="N8" s="8">
-        <v>3600</v>
-      </c>
-      <c r="O8" s="8">
+      <c r="N8">
+        <v>3600</v>
+      </c>
+      <c r="O8">
         <v>25.528300000000002</v>
       </c>
-      <c r="P8" s="8">
+      <c r="P8">
         <v>115080</v>
       </c>
-      <c r="R8" s="8">
+      <c r="R8">
         <v>399.45600000000002</v>
       </c>
-      <c r="S8" s="8">
-        <v>3600</v>
-      </c>
-      <c r="T8" s="8">
+      <c r="S8">
+        <v>3600</v>
+      </c>
+      <c r="T8">
         <v>44.290999999999997</v>
       </c>
-      <c r="U8" s="8">
+      <c r="U8">
         <v>41960</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" t="s">
         <v>317</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9">
         <v>844.22900000000004</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9">
         <v>676.19</v>
       </c>
-      <c r="E9" s="8">
-        <v>0</v>
-      </c>
-      <c r="F9" s="8">
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
         <v>627</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9">
         <v>844.22900000000004</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9">
         <v>455.69499999999999</v>
       </c>
-      <c r="J9" s="8">
-        <v>0</v>
-      </c>
-      <c r="K9" s="8">
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
         <v>814</v>
       </c>
-      <c r="M9" s="8">
+      <c r="M9">
         <v>987.04300000000001</v>
       </c>
-      <c r="N9" s="8">
-        <v>3600</v>
-      </c>
-      <c r="O9" s="8">
+      <c r="N9">
+        <v>3600</v>
+      </c>
+      <c r="O9">
         <v>23.322399999999998</v>
       </c>
-      <c r="P9" s="8">
+      <c r="P9">
         <v>3512</v>
       </c>
-      <c r="R9" s="8">
+      <c r="R9">
         <v>882.53700000000003</v>
       </c>
-      <c r="S9" s="8">
-        <v>3600</v>
-      </c>
-      <c r="T9" s="8">
+      <c r="S9">
+        <v>3600</v>
+      </c>
+      <c r="T9">
         <v>36.292099999999998</v>
       </c>
-      <c r="U9" s="8">
+      <c r="U9">
         <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" t="s">
         <v>318</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10">
         <v>514.65200000000004</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10">
         <v>1.54</v>
       </c>
-      <c r="E10" s="8">
-        <v>0</v>
-      </c>
-      <c r="F10" s="8">
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
         <v>949</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10">
         <v>514.65200000000004</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10">
         <v>1.8149999999999999</v>
       </c>
-      <c r="J10" s="8">
-        <v>0</v>
-      </c>
-      <c r="K10" s="8">
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
         <v>1180</v>
       </c>
-      <c r="M10" s="8">
+      <c r="M10">
         <v>506.71199999999999</v>
       </c>
-      <c r="N10" s="8">
-        <v>3600</v>
-      </c>
-      <c r="O10" s="8">
+      <c r="N10">
+        <v>3600</v>
+      </c>
+      <c r="O10">
         <v>10.269399999999999</v>
       </c>
-      <c r="P10" s="8">
+      <c r="P10">
         <v>506826</v>
       </c>
-      <c r="R10" s="8">
+      <c r="R10">
         <v>455.06400000000002</v>
       </c>
-      <c r="S10" s="8">
-        <v>3600</v>
-      </c>
-      <c r="T10" s="8">
+      <c r="S10">
+        <v>3600</v>
+      </c>
+      <c r="T10">
         <v>47.806699999999999</v>
       </c>
-      <c r="U10" s="8">
+      <c r="U10">
         <v>187141</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" t="s">
         <v>319</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11">
         <v>229.25700000000001</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11">
         <v>1.286</v>
       </c>
-      <c r="E11" s="8">
-        <v>0</v>
-      </c>
-      <c r="F11" s="8">
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
         <v>1293</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11">
         <v>225.65799999999999</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11">
         <v>0.54200000000000004</v>
       </c>
-      <c r="J11" s="8">
-        <v>0</v>
-      </c>
-      <c r="K11" s="8">
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
         <v>478</v>
       </c>
-      <c r="M11" s="8">
+      <c r="M11">
         <v>213.864</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11">
         <v>11.058999999999999</v>
       </c>
-      <c r="O11" s="8">
-        <v>0</v>
-      </c>
-      <c r="P11" s="8">
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
         <v>2692</v>
       </c>
-      <c r="R11" s="8">
+      <c r="R11">
         <v>212.001</v>
       </c>
-      <c r="S11" s="8">
+      <c r="S11">
         <v>1054.6300000000001</v>
       </c>
-      <c r="T11" s="8">
-        <v>0</v>
-      </c>
-      <c r="U11" s="8">
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
         <v>44738</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" t="s">
         <v>320</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12">
         <v>234.364</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12">
         <v>9.0139999999999993</v>
       </c>
-      <c r="E12" s="8">
-        <v>0</v>
-      </c>
-      <c r="F12" s="8">
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
         <v>6434</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12">
         <v>234.364</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12">
         <v>4.726</v>
       </c>
-      <c r="J12" s="8">
-        <v>0</v>
-      </c>
-      <c r="K12" s="8">
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
         <v>3111</v>
       </c>
-      <c r="M12" s="8">
+      <c r="M12">
         <v>227.75899999999999</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N12">
         <v>170.96299999999999</v>
       </c>
-      <c r="O12" s="8">
-        <v>0</v>
-      </c>
-      <c r="P12" s="8">
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
         <v>23394</v>
       </c>
-      <c r="R12" s="8">
+      <c r="R12">
         <v>225.89099999999999</v>
       </c>
-      <c r="S12" s="8">
-        <v>3600</v>
-      </c>
-      <c r="T12" s="8">
+      <c r="S12">
+        <v>3600</v>
+      </c>
+      <c r="T12">
         <v>8.0391499999999994</v>
       </c>
-      <c r="U12" s="8">
+      <c r="U12">
         <v>94297</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" t="s">
         <v>321</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13">
         <v>220.55099999999999</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13">
         <v>0.23</v>
       </c>
-      <c r="E13" s="8">
-        <v>0</v>
-      </c>
-      <c r="F13" s="8">
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
         <v>98</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13">
         <v>220.55099999999999</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13">
         <v>0.19700000000000001</v>
       </c>
-      <c r="J13" s="8">
-        <v>0</v>
-      </c>
-      <c r="K13" s="8">
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
         <v>93</v>
       </c>
-      <c r="M13" s="8">
+      <c r="M13">
         <v>220.55099999999999</v>
       </c>
-      <c r="N13" s="8">
+      <c r="N13">
         <v>79.018000000000001</v>
       </c>
-      <c r="O13" s="8">
-        <v>0</v>
-      </c>
-      <c r="P13" s="8">
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
         <v>7863</v>
       </c>
-      <c r="R13" s="8">
+      <c r="R13">
         <v>219.512</v>
       </c>
-      <c r="S13" s="8">
-        <v>3600</v>
-      </c>
-      <c r="T13" s="8">
+      <c r="S13">
+        <v>3600</v>
+      </c>
+      <c r="T13">
         <v>5.1528999999999998</v>
       </c>
-      <c r="U13" s="8">
+      <c r="U13">
         <v>91833</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" t="s">
         <v>322</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14">
         <v>232.738</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14">
         <v>8.5350000000000001</v>
       </c>
-      <c r="E14" s="8">
-        <v>0</v>
-      </c>
-      <c r="F14" s="8">
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
         <v>5938</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14">
         <v>232.738</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14">
         <v>4.9480000000000004</v>
       </c>
-      <c r="J14" s="8">
-        <v>0</v>
-      </c>
-      <c r="K14" s="8">
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
         <v>3354</v>
       </c>
-      <c r="M14" s="8">
+      <c r="M14">
         <v>232.738</v>
       </c>
-      <c r="N14" s="8">
+      <c r="N14">
         <v>1333.36</v>
       </c>
-      <c r="O14" s="8">
-        <v>0</v>
-      </c>
-      <c r="P14" s="8">
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
         <v>76524</v>
       </c>
-      <c r="R14" s="8">
+      <c r="R14">
         <v>230.88800000000001</v>
       </c>
-      <c r="S14" s="8">
-        <v>3600</v>
-      </c>
-      <c r="T14" s="8">
+      <c r="S14">
+        <v>3600</v>
+      </c>
+      <c r="T14">
         <v>9.2630300000000005</v>
       </c>
-      <c r="U14" s="8">
+      <c r="U14">
         <v>78899</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" t="s">
         <v>323</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15">
         <v>618.24099999999999</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15">
         <v>355.69299999999998</v>
       </c>
-      <c r="E15" s="8">
-        <v>0</v>
-      </c>
-      <c r="F15" s="8">
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
         <v>2113</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15">
         <v>592.46</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15">
         <v>11.127000000000001</v>
       </c>
-      <c r="J15" s="8">
-        <v>0</v>
-      </c>
-      <c r="K15" s="8">
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
         <v>25</v>
       </c>
-      <c r="M15" s="8">
+      <c r="M15">
         <v>649.24199999999996</v>
       </c>
-      <c r="N15" s="8">
-        <v>3600</v>
-      </c>
-      <c r="O15" s="8">
+      <c r="N15">
+        <v>3600</v>
+      </c>
+      <c r="O15">
         <v>30.464500000000001</v>
       </c>
-      <c r="P15" s="8">
+      <c r="P15">
         <v>6617</v>
       </c>
-      <c r="R15" s="8">
+      <c r="R15">
         <v>599.35199999999998</v>
       </c>
-      <c r="S15" s="8">
-        <v>3600</v>
-      </c>
-      <c r="T15" s="8">
+      <c r="S15">
+        <v>3600</v>
+      </c>
+      <c r="T15">
         <v>52.969499999999996</v>
       </c>
-      <c r="U15" s="8">
+      <c r="U15">
         <v>634</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" t="s">
         <v>324</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16">
         <v>475.738</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16">
         <v>51.366</v>
       </c>
-      <c r="E16" s="8">
-        <v>0</v>
-      </c>
-      <c r="F16" s="8">
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
         <v>6381</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16">
         <v>475.738</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16">
         <v>52.470999999999997</v>
       </c>
-      <c r="J16" s="8">
-        <v>0</v>
-      </c>
-      <c r="K16" s="8">
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
         <v>7060</v>
       </c>
-      <c r="M16" s="8">
+      <c r="M16">
         <v>525.20399999999995</v>
       </c>
-      <c r="N16" s="8">
-        <v>3600</v>
-      </c>
-      <c r="O16" s="8">
+      <c r="N16">
+        <v>3600</v>
+      </c>
+      <c r="O16">
         <v>20.315300000000001</v>
       </c>
-      <c r="P16" s="8">
+      <c r="P16">
         <v>71299</v>
       </c>
-      <c r="R16" s="8">
+      <c r="R16">
         <v>486.10500000000002</v>
       </c>
-      <c r="S16" s="8">
-        <v>3600</v>
-      </c>
-      <c r="T16" s="8">
+      <c r="S16">
+        <v>3600</v>
+      </c>
+      <c r="T16">
         <v>24.297899999999998</v>
       </c>
-      <c r="U16" s="8">
+      <c r="U16">
         <v>25495</v>
       </c>
     </row>
@@ -18468,8 +18463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5E210A-AC17-48CD-AA59-D950944C690E}">
   <dimension ref="A1:P298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
-      <selection activeCell="A300" sqref="A300:XFD300"/>
+    <sheetView topLeftCell="A268" workbookViewId="0">
+      <selection activeCell="U284" sqref="U284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18482,25 +18477,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="D1" s="5"/>
+      <c r="F1" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="J1" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="N1" s="1" t="s">
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="N1" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">

</xml_diff>